<commit_message>
Order by date correctly
</commit_message>
<xml_diff>
--- a/data/fga-eps-mds-2020-2-Projeto-Kokama-qualidade-total-produto-20-5-2021-00:00.xlsx
+++ b/data/fga-eps-mds-2020-2-Projeto-Kokama-qualidade-total-produto-20-5-2021-00:00.xlsx
@@ -16,7 +16,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -55,11 +58,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -482,10 +486,10 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0.1904761904761905</v>
+        <v>0.1739130434782609</v>
       </c>
       <c r="B2" t="n">
-        <v>0.09523809523809523</v>
+        <v>0.08695652173913043</v>
       </c>
       <c r="C2" t="n">
         <v>1</v>
@@ -495,30 +499,28 @@
           <t>2020_2-Projeto-Kokama-Traducao</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>05-04-2021</t>
-        </is>
+      <c r="E2" s="2" t="n">
+        <v>44278</v>
       </c>
       <c r="F2" t="n">
-        <v>465</v>
+        <v>336</v>
       </c>
       <c r="G2" t="n">
-        <v>0.4242857142857143</v>
+        <v>0.4160869565217392</v>
       </c>
       <c r="H2" t="n">
-        <v>0.4242857142857143</v>
+        <v>0.4160869565217392</v>
       </c>
       <c r="I2" t="n">
-        <v>0.4242857142857143</v>
+        <v>0.4160869565217392</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>0.2857142857142857</v>
+        <v>0.1904761904761905</v>
       </c>
       <c r="B3" t="n">
-        <v>0.1428571428571428</v>
+        <v>0.09523809523809523</v>
       </c>
       <c r="C3" t="n">
         <v>1</v>
@@ -528,22 +530,20 @@
           <t>2020_2-Projeto-Kokama-Traducao</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>06-04-2021</t>
-        </is>
+      <c r="E3" s="2" t="n">
+        <v>44291</v>
       </c>
       <c r="F3" t="n">
-        <v>308</v>
+        <v>465</v>
       </c>
       <c r="G3" t="n">
-        <v>0.4714285714285714</v>
+        <v>0.4242857142857143</v>
       </c>
       <c r="H3" t="n">
-        <v>0.4714285714285714</v>
+        <v>0.4242857142857143</v>
       </c>
       <c r="I3" t="n">
-        <v>0.4714285714285714</v>
+        <v>0.4242857142857143</v>
       </c>
     </row>
     <row r="4">
@@ -561,13 +561,11 @@
           <t>2020_2-Projeto-Kokama-Traducao</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>14-05-2021</t>
-        </is>
+      <c r="E4" s="2" t="n">
+        <v>44292</v>
       </c>
       <c r="F4" t="n">
-        <v>330</v>
+        <v>308</v>
       </c>
       <c r="G4" t="n">
         <v>0.4714285714285714</v>
@@ -581,10 +579,10 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>0.1739130434782609</v>
+        <v>0.2857142857142857</v>
       </c>
       <c r="B5" t="n">
-        <v>0.08695652173913043</v>
+        <v>0.1428571428571428</v>
       </c>
       <c r="C5" t="n">
         <v>1</v>
@@ -594,30 +592,28 @@
           <t>2020_2-Projeto-Kokama-Traducao</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>23-03-2021</t>
-        </is>
+      <c r="E5" s="2" t="n">
+        <v>44330</v>
       </c>
       <c r="F5" t="n">
-        <v>336</v>
+        <v>330</v>
       </c>
       <c r="G5" t="n">
-        <v>0.4160869565217392</v>
+        <v>0.4714285714285714</v>
       </c>
       <c r="H5" t="n">
-        <v>0.4160869565217392</v>
+        <v>0.4714285714285714</v>
       </c>
       <c r="I5" t="n">
-        <v>0.4160869565217392</v>
+        <v>0.4714285714285714</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="B6" t="n">
-        <v>0.08</v>
+        <v>0</v>
       </c>
       <c r="C6" t="n">
         <v>1</v>
@@ -627,22 +623,20 @@
           <t>2020_2-Projeto-Kokama-Usuario</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>14-05-2021</t>
-        </is>
+      <c r="E6" s="2" t="n">
+        <v>44303</v>
       </c>
       <c r="F6" t="n">
-        <v>570</v>
+        <v>24</v>
       </c>
       <c r="G6" t="n">
-        <v>0.4224</v>
+        <v>0.33</v>
       </c>
       <c r="H6" t="n">
-        <v>0.4224</v>
+        <v>0.33</v>
       </c>
       <c r="I6" t="n">
-        <v>0.4224</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="7">
@@ -660,13 +654,11 @@
           <t>2020_2-Projeto-Kokama-Usuario</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>15-05-2021</t>
-        </is>
+      <c r="E7" s="2" t="n">
+        <v>44330</v>
       </c>
       <c r="F7" t="n">
-        <v>531</v>
+        <v>570</v>
       </c>
       <c r="G7" t="n">
         <v>0.4224</v>
@@ -680,10 +672,10 @@
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>0.3043478260869565</v>
+        <v>0.2</v>
       </c>
       <c r="B8" t="n">
-        <v>0.1304347826086956</v>
+        <v>0.08</v>
       </c>
       <c r="C8" t="n">
         <v>1</v>
@@ -693,30 +685,28 @@
           <t>2020_2-Projeto-Kokama-Usuario</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>16-05-2021</t>
-        </is>
+      <c r="E8" s="2" t="n">
+        <v>44331</v>
       </c>
       <c r="F8" t="n">
-        <v>687</v>
+        <v>531</v>
       </c>
       <c r="G8" t="n">
-        <v>0.4734782608695652</v>
+        <v>0.4224</v>
       </c>
       <c r="H8" t="n">
-        <v>0.4734782608695652</v>
+        <v>0.4224</v>
       </c>
       <c r="I8" t="n">
-        <v>0.4734782608695652</v>
+        <v>0.4224</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>0</v>
+        <v>0.3043478260869565</v>
       </c>
       <c r="B9" t="n">
-        <v>0</v>
+        <v>0.1304347826086956</v>
       </c>
       <c r="C9" t="n">
         <v>1</v>
@@ -726,22 +716,20 @@
           <t>2020_2-Projeto-Kokama-Usuario</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>17-04-2021</t>
-        </is>
+      <c r="E9" s="2" t="n">
+        <v>44332</v>
       </c>
       <c r="F9" t="n">
-        <v>24</v>
+        <v>687</v>
       </c>
       <c r="G9" t="n">
-        <v>0.33</v>
+        <v>0.4734782608695652</v>
       </c>
       <c r="H9" t="n">
-        <v>0.33</v>
+        <v>0.4734782608695652</v>
       </c>
       <c r="I9" t="n">
-        <v>0.33</v>
+        <v>0.4734782608695652</v>
       </c>
     </row>
     <row r="10">
@@ -759,10 +747,8 @@
           <t>2020_2-Projeto-Kokama-Ensino</t>
         </is>
       </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>14-04-2021</t>
-        </is>
+      <c r="E10" s="2" t="n">
+        <v>44300</v>
       </c>
       <c r="F10" t="n">
         <v>371</v>
@@ -792,10 +778,8 @@
           <t>2020_2-Projeto-Kokama-Ensino</t>
         </is>
       </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>14-05-2021</t>
-        </is>
+      <c r="E11" s="2" t="n">
+        <v>44330</v>
       </c>
       <c r="F11" t="n">
         <v>332</v>
@@ -825,10 +809,8 @@
           <t>2020_2-Projeto-Kokama-Ensino</t>
         </is>
       </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>15-05-2021</t>
-        </is>
+      <c r="E12" s="2" t="n">
+        <v>44331</v>
       </c>
       <c r="F12" t="n">
         <v>359</v>
@@ -845,10 +827,10 @@
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>0.5454545454545454</v>
+        <v>0.5</v>
       </c>
       <c r="B13" t="n">
-        <v>0.04545454545454546</v>
+        <v>0</v>
       </c>
       <c r="C13" t="n">
         <v>1</v>
@@ -858,30 +840,28 @@
           <t>2020_2-Projeto-Kokama-Front-end</t>
         </is>
       </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>05-04-2021</t>
-        </is>
+      <c r="E13" s="2" t="n">
+        <v>44278</v>
       </c>
       <c r="F13" t="n">
-        <v>1071</v>
+        <v>429</v>
       </c>
       <c r="G13" t="n">
-        <v>0.525</v>
+        <v>0.495</v>
       </c>
       <c r="H13" t="n">
-        <v>0.525</v>
+        <v>0.495</v>
       </c>
       <c r="I13" t="n">
-        <v>0.525</v>
+        <v>0.495</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>0.5151515151515151</v>
+        <v>0.5454545454545454</v>
       </c>
       <c r="B14" t="n">
-        <v>0.0303030303030303</v>
+        <v>0.04545454545454546</v>
       </c>
       <c r="C14" t="n">
         <v>1</v>
@@ -891,30 +871,28 @@
           <t>2020_2-Projeto-Kokama-Front-end</t>
         </is>
       </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>11-05-2021</t>
-        </is>
+      <c r="E14" s="2" t="n">
+        <v>44291</v>
       </c>
       <c r="F14" t="n">
-        <v>1628</v>
+        <v>1071</v>
       </c>
       <c r="G14" t="n">
-        <v>0.51</v>
+        <v>0.525</v>
       </c>
       <c r="H14" t="n">
-        <v>0.51</v>
+        <v>0.525</v>
       </c>
       <c r="I14" t="n">
-        <v>0.51</v>
+        <v>0.525</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>0.5600000000000001</v>
+        <v>0.5151515151515151</v>
       </c>
       <c r="B15" t="n">
-        <v>0.04</v>
+        <v>0.0303030303030303</v>
       </c>
       <c r="C15" t="n">
         <v>1</v>
@@ -924,30 +902,28 @@
           <t>2020_2-Projeto-Kokama-Front-end</t>
         </is>
       </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>12-05-2021</t>
-        </is>
+      <c r="E15" s="2" t="n">
+        <v>44327</v>
       </c>
       <c r="F15" t="n">
-        <v>1160</v>
+        <v>1628</v>
       </c>
       <c r="G15" t="n">
-        <v>0.528</v>
+        <v>0.51</v>
       </c>
       <c r="H15" t="n">
-        <v>0.528</v>
+        <v>0.51</v>
       </c>
       <c r="I15" t="n">
-        <v>0.528</v>
+        <v>0.51</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>0.5151515151515151</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="B16" t="n">
-        <v>0</v>
+        <v>0.04</v>
       </c>
       <c r="C16" t="n">
         <v>1</v>
@@ -957,22 +933,20 @@
           <t>2020_2-Projeto-Kokama-Front-end</t>
         </is>
       </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>15-05-2021</t>
-        </is>
+      <c r="E16" s="2" t="n">
+        <v>44328</v>
       </c>
       <c r="F16" t="n">
-        <v>1673</v>
+        <v>1160</v>
       </c>
       <c r="G16" t="n">
-        <v>0.5</v>
+        <v>0.528</v>
       </c>
       <c r="H16" t="n">
-        <v>0.5</v>
+        <v>0.528</v>
       </c>
       <c r="I16" t="n">
-        <v>0.5</v>
+        <v>0.528</v>
       </c>
     </row>
     <row r="17">
@@ -980,7 +954,7 @@
         <v>0.5151515151515151</v>
       </c>
       <c r="B17" t="n">
-        <v>0.0303030303030303</v>
+        <v>0</v>
       </c>
       <c r="C17" t="n">
         <v>1</v>
@@ -990,30 +964,28 @@
           <t>2020_2-Projeto-Kokama-Front-end</t>
         </is>
       </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>20-05-2021</t>
-        </is>
+      <c r="E17" s="2" t="n">
+        <v>44331</v>
       </c>
       <c r="F17" t="n">
-        <v>1627</v>
+        <v>1673</v>
       </c>
       <c r="G17" t="n">
-        <v>0.51</v>
+        <v>0.5</v>
       </c>
       <c r="H17" t="n">
-        <v>0.51</v>
+        <v>0.5</v>
       </c>
       <c r="I17" t="n">
-        <v>0.51</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>0.5</v>
+        <v>0.5151515151515151</v>
       </c>
       <c r="B18" t="n">
-        <v>0</v>
+        <v>0.0303030303030303</v>
       </c>
       <c r="C18" t="n">
         <v>1</v>
@@ -1023,22 +995,20 @@
           <t>2020_2-Projeto-Kokama-Front-end</t>
         </is>
       </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>23-03-2021</t>
-        </is>
+      <c r="E18" s="2" t="n">
+        <v>44336</v>
       </c>
       <c r="F18" t="n">
-        <v>429</v>
+        <v>1627</v>
       </c>
       <c r="G18" t="n">
-        <v>0.495</v>
+        <v>0.51</v>
       </c>
       <c r="H18" t="n">
-        <v>0.495</v>
+        <v>0.51</v>
       </c>
       <c r="I18" t="n">
-        <v>0.495</v>
+        <v>0.51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>